<commit_message>
results from testing MoC package
</commit_message>
<xml_diff>
--- a/Test_excel_name.xlsx
+++ b/Test_excel_name.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\milkg\EESI\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B1EC261-AEBA-41DF-8798-36EEEF97CBA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="2976" yWindow="240" windowWidth="14688" windowHeight="11136" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="True Positives" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
     <sheet name="Precision" sheetId="5" r:id="rId5"/>
     <sheet name="Recall" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -69,8 +75,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,6 +139,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -179,7 +193,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -211,9 +225,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -245,6 +277,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -420,14 +470,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="7" max="7" width="13" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -444,7 +499,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -464,7 +519,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -484,7 +539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -504,7 +559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -524,7 +579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -544,7 +599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -564,7 +619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -590,14 +645,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -614,7 +669,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -634,7 +689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -654,7 +709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -674,7 +729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -694,7 +749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -714,7 +769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -734,7 +789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -760,14 +815,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -784,7 +839,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -804,7 +859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -824,7 +879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -844,7 +899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -864,7 +919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -884,7 +939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -904,7 +959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -930,14 +985,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -954,7 +1009,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -974,7 +1029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -994,7 +1049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1014,7 +1069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1034,7 +1089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1054,7 +1109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1074,7 +1129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1100,14 +1155,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1118,7 +1173,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1132,7 +1187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1146,7 +1201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1160,7 +1215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1174,7 +1229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1188,7 +1243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1202,7 +1257,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1222,14 +1277,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1240,7 +1295,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1254,7 +1309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1268,7 +1323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1282,7 +1337,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1296,7 +1351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1310,7 +1365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1324,7 +1379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>

</xml_diff>